<commit_message>
Fixed glitch in data sample selection code
</commit_message>
<xml_diff>
--- a/helperfiles/Prey_Classes.xlsx
+++ b/helperfiles/Prey_Classes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/26362cec7e0913ab/Documents/Nhydra/Projects/SOFA2/SOFA/helperfiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{062BBBD3-4C41-4C14-9D50-3729DAC20B28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7FF3D1DC-8CCA-440A-B013-C1849193E3C6}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{062BBBD3-4C41-4C14-9D50-3729DAC20B28}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2EA3348D-B66D-40AA-9528-D839A32D64D3}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1440" windowWidth="24150" windowHeight="14760" xr2:uid="{B205C025-E4C6-4B35-B9D4-36F7EDCDF466}"/>
+    <workbookView xWindow="1635" yWindow="990" windowWidth="26850" windowHeight="13365" xr2:uid="{B205C025-E4C6-4B35-B9D4-36F7EDCDF466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>other_crab</t>
   </si>
   <si>
-    <t>un-id crabs and vaious scrab sp</t>
-  </si>
-  <si>
     <t>snail</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>Lobster (southern CA only)</t>
+  </si>
+  <si>
+    <t>crabs, various sp</t>
   </si>
 </sst>
 </file>
@@ -501,7 +501,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +584,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -592,10 +592,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -603,10 +603,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -614,10 +614,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -625,10 +625,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -636,10 +636,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -647,10 +647,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -658,10 +658,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,10 +669,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -680,10 +680,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
         <v>31</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>